<commit_message>
Import all string fields. Issues with dates...
</commit_message>
<xml_diff>
--- a/platform/src/test/resources/excel/employees-to-import.xlsx
+++ b/platform/src/test/resources/excel/employees-to-import.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\stm\hreasy\src\hreasy\platform\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\stm\hreasy\src\hreasy\platform\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{301EDB49-11FC-463B-9791-CE0140600F63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC767816-270A-4833-A430-5876FC8B57FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TDSheet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="60">
   <si>
     <t>Личные данные сотрудников</t>
   </si>
@@ -65,18 +65,12 @@
     <t>Дата увольнения</t>
   </si>
   <si>
-    <t>График работы</t>
-  </si>
-  <si>
     <t>Дата рождения</t>
   </si>
   <si>
     <t>Пол</t>
   </si>
   <si>
-    <t>Удостоверение личности</t>
-  </si>
-  <si>
     <t>Адрес места проживания</t>
   </si>
   <si>
@@ -95,9 +89,6 @@
     <t>Состав семьи</t>
   </si>
   <si>
-    <t>Вид</t>
-  </si>
-  <si>
     <t>Серия</t>
   </si>
   <si>
@@ -110,27 +101,6 @@
     <t>Кем выдано</t>
   </si>
   <si>
-    <t>Код подразделения</t>
-  </si>
-  <si>
-    <t>01.10.2020</t>
-  </si>
-  <si>
-    <t>Основной график</t>
-  </si>
-  <si>
-    <t>14.07.1995</t>
-  </si>
-  <si>
-    <t>Женский</t>
-  </si>
-  <si>
-    <t>Паспорт гражданина РФ</t>
-  </si>
-  <si>
-    <t>13.08.2019</t>
-  </si>
-  <si>
     <t>ГУ МВД России по Нижегородской области</t>
   </si>
   <si>
@@ -158,15 +128,6 @@
     <t>Никогда не состоял(а) в браке</t>
   </si>
   <si>
-    <t>28.03.2022</t>
-  </si>
-  <si>
-    <t>08.06.1993</t>
-  </si>
-  <si>
-    <t>20.09.2022</t>
-  </si>
-  <si>
     <t>ООО "Тестовая"</t>
   </si>
   <si>
@@ -179,9 +140,6 @@
     <t>ГУ МВД России</t>
   </si>
   <si>
-    <t>500-000</t>
-  </si>
-  <si>
     <t>РОССИЯ, 602222, Лучший город на свете, супер улица</t>
   </si>
   <si>
@@ -221,12 +179,6 @@
     <t>Непонятный отдел</t>
   </si>
   <si>
-    <t>500-001</t>
-  </si>
-  <si>
-    <t>500-002</t>
-  </si>
-  <si>
     <t>Сын:Ванька</t>
   </si>
   <si>
@@ -243,6 +195,12 @@
   </si>
   <si>
     <t>87 21</t>
+  </si>
+  <si>
+    <t>женский</t>
+  </si>
+  <si>
+    <t>Муж.</t>
   </si>
 </sst>
 </file>
@@ -396,6 +354,24 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -405,31 +381,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -775,13 +733,13 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr autoPageBreaks="0" fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AZ14"/>
+  <dimension ref="A1:AW14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AI1" workbookViewId="0">
-      <selection activeCell="AQ14" sqref="AQ14"/>
+    <sheetView tabSelected="1" topLeftCell="AH1" workbookViewId="0">
+      <selection activeCell="AL11" sqref="AL11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="11.45" customHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="11.45" customHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.83203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="3.6640625" style="1" customWidth="1"/>
@@ -802,25 +760,20 @@
     <col min="33" max="33" width="21.1640625" style="1" customWidth="1"/>
     <col min="34" max="34" width="52.5" style="1" customWidth="1"/>
     <col min="35" max="35" width="35" style="1" customWidth="1"/>
-    <col min="36" max="37" width="14" style="1" customWidth="1"/>
-    <col min="38" max="38" width="31.5" style="1" customWidth="1"/>
-    <col min="39" max="39" width="14" style="1" customWidth="1"/>
-    <col min="40" max="40" width="10.6640625" style="1" customWidth="1"/>
-    <col min="41" max="41" width="26.83203125" style="1" customWidth="1"/>
-    <col min="42" max="42" width="9.33203125" style="1" customWidth="1"/>
-    <col min="43" max="43" width="11.6640625" style="1" customWidth="1"/>
-    <col min="44" max="44" width="14" style="1" customWidth="1"/>
-    <col min="45" max="45" width="74.6640625" style="1" customWidth="1"/>
-    <col min="46" max="46" width="18.1640625" style="1" customWidth="1"/>
-    <col min="47" max="47" width="74.6640625" style="1" customWidth="1"/>
-    <col min="48" max="48" width="57.1640625" style="1" customWidth="1"/>
-    <col min="49" max="50" width="17.5" style="1" customWidth="1"/>
-    <col min="51" max="51" width="14.33203125" style="1" customWidth="1"/>
-    <col min="52" max="52" width="74.6640625" style="1" customWidth="1"/>
+    <col min="36" max="38" width="14" style="1" customWidth="1"/>
+    <col min="39" max="39" width="10.6640625" style="1" customWidth="1"/>
+    <col min="40" max="40" width="9.33203125" style="1" customWidth="1"/>
+    <col min="41" max="41" width="11.6640625" style="1" customWidth="1"/>
+    <col min="42" max="42" width="14" style="1" customWidth="1"/>
+    <col min="43" max="44" width="74.6640625" style="1" customWidth="1"/>
+    <col min="45" max="45" width="57.1640625" style="1" customWidth="1"/>
+    <col min="46" max="47" width="17.5" style="1" customWidth="1"/>
+    <col min="48" max="48" width="14.33203125" style="1" customWidth="1"/>
+    <col min="49" max="49" width="74.6640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:52" s="1" customFormat="1" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:52" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:49" s="1" customFormat="1" ht="10.15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="1:49" ht="25.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -842,285 +795,271 @@
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
     </row>
-    <row r="3" spans="1:52" s="1" customFormat="1" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:52" ht="26" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:49" s="1" customFormat="1" ht="10.15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="1:49" ht="26.1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="3"/>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="8"/>
+      <c r="D4" s="14"/>
     </row>
-    <row r="5" spans="1:52" s="1" customFormat="1" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:52" ht="13.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="9" t="s">
+    <row r="5" spans="1:49" s="1" customFormat="1" ht="10.15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="6" spans="1:49" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
-      <c r="K6" s="9"/>
-      <c r="L6" s="9"/>
-      <c r="M6" s="9"/>
-      <c r="N6" s="9"/>
-      <c r="O6" s="9"/>
-      <c r="P6" s="9"/>
-      <c r="Q6" s="9"/>
-      <c r="R6" s="9"/>
-      <c r="S6" s="9"/>
-      <c r="T6" s="9"/>
-      <c r="U6" s="9"/>
-      <c r="V6" s="9"/>
-      <c r="W6" s="9"/>
-      <c r="X6" s="9"/>
-      <c r="Y6" s="9"/>
-      <c r="Z6" s="9"/>
-      <c r="AA6" s="9"/>
-      <c r="AB6" s="9"/>
-      <c r="AC6" s="9"/>
-      <c r="AD6" s="9"/>
-      <c r="AE6" s="9"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="15"/>
+      <c r="N6" s="15"/>
+      <c r="O6" s="15"/>
+      <c r="P6" s="15"/>
+      <c r="Q6" s="15"/>
+      <c r="R6" s="15"/>
+      <c r="S6" s="15"/>
+      <c r="T6" s="15"/>
+      <c r="U6" s="15"/>
+      <c r="V6" s="15"/>
+      <c r="W6" s="15"/>
+      <c r="X6" s="15"/>
+      <c r="Y6" s="15"/>
+      <c r="Z6" s="15"/>
+      <c r="AA6" s="15"/>
+      <c r="AB6" s="15"/>
+      <c r="AC6" s="15"/>
+      <c r="AD6" s="15"/>
+      <c r="AE6" s="15"/>
     </row>
-    <row r="7" spans="1:52" ht="13.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="9" t="s">
+    <row r="7" spans="1:49" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="10">
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="16">
         <v>3</v>
       </c>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
-      <c r="L7" s="10"/>
-      <c r="M7" s="10"/>
-      <c r="N7" s="10"/>
-      <c r="O7" s="10"/>
-      <c r="P7" s="10"/>
-      <c r="Q7" s="10"/>
-      <c r="R7" s="10"/>
-      <c r="S7" s="10"/>
-      <c r="T7" s="10"/>
-      <c r="U7" s="10"/>
-      <c r="V7" s="10"/>
-      <c r="W7" s="10"/>
-      <c r="X7" s="10"/>
-      <c r="Y7" s="10"/>
-      <c r="Z7" s="10"/>
-      <c r="AA7" s="10"/>
-      <c r="AB7" s="10"/>
-      <c r="AC7" s="10"/>
-      <c r="AD7" s="10"/>
-      <c r="AE7" s="10"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="16"/>
+      <c r="K7" s="16"/>
+      <c r="L7" s="16"/>
+      <c r="M7" s="16"/>
+      <c r="N7" s="16"/>
+      <c r="O7" s="16"/>
+      <c r="P7" s="16"/>
+      <c r="Q7" s="16"/>
+      <c r="R7" s="16"/>
+      <c r="S7" s="16"/>
+      <c r="T7" s="16"/>
+      <c r="U7" s="16"/>
+      <c r="V7" s="16"/>
+      <c r="W7" s="16"/>
+      <c r="X7" s="16"/>
+      <c r="Y7" s="16"/>
+      <c r="Z7" s="16"/>
+      <c r="AA7" s="16"/>
+      <c r="AB7" s="16"/>
+      <c r="AC7" s="16"/>
+      <c r="AD7" s="16"/>
+      <c r="AE7" s="16"/>
     </row>
-    <row r="8" spans="1:52" s="1" customFormat="1" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="10"/>
-      <c r="M8" s="10"/>
-      <c r="N8" s="10"/>
-      <c r="O8" s="10"/>
-      <c r="P8" s="10"/>
-      <c r="Q8" s="10"/>
-      <c r="R8" s="10"/>
-      <c r="S8" s="10"/>
-      <c r="T8" s="10"/>
-      <c r="U8" s="10"/>
-      <c r="V8" s="10"/>
-      <c r="W8" s="10"/>
-      <c r="X8" s="10"/>
-      <c r="Y8" s="10"/>
-      <c r="Z8" s="10"/>
-      <c r="AA8" s="10"/>
-      <c r="AB8" s="10"/>
-      <c r="AC8" s="10"/>
-      <c r="AD8" s="10"/>
-      <c r="AE8" s="10"/>
+    <row r="8" spans="1:49" s="1" customFormat="1" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="16"/>
+      <c r="L8" s="16"/>
+      <c r="M8" s="16"/>
+      <c r="N8" s="16"/>
+      <c r="O8" s="16"/>
+      <c r="P8" s="16"/>
+      <c r="Q8" s="16"/>
+      <c r="R8" s="16"/>
+      <c r="S8" s="16"/>
+      <c r="T8" s="16"/>
+      <c r="U8" s="16"/>
+      <c r="V8" s="16"/>
+      <c r="W8" s="16"/>
+      <c r="X8" s="16"/>
+      <c r="Y8" s="16"/>
+      <c r="Z8" s="16"/>
+      <c r="AA8" s="16"/>
+      <c r="AB8" s="16"/>
+      <c r="AC8" s="16"/>
+      <c r="AD8" s="16"/>
+      <c r="AE8" s="16"/>
     </row>
-    <row r="9" spans="1:52" ht="13.05" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="11" t="s">
+    <row r="9" spans="1:49" ht="13.15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11" t="s">
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="I9" s="11"/>
-      <c r="J9" s="11"/>
-      <c r="K9" s="11"/>
-      <c r="L9" s="11"/>
-      <c r="M9" s="11"/>
-      <c r="N9" s="11"/>
-      <c r="O9" s="11"/>
-      <c r="P9" s="11"/>
-      <c r="Q9" s="11" t="s">
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="9"/>
+      <c r="P9" s="9"/>
+      <c r="Q9" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="R9" s="11"/>
-      <c r="S9" s="11"/>
-      <c r="T9" s="11"/>
-      <c r="U9" s="11"/>
-      <c r="V9" s="11"/>
-      <c r="W9" s="11"/>
-      <c r="X9" s="11"/>
-      <c r="Y9" s="11"/>
-      <c r="Z9" s="11"/>
-      <c r="AA9" s="11"/>
-      <c r="AB9" s="11"/>
-      <c r="AC9" s="11"/>
-      <c r="AD9" s="11"/>
-      <c r="AE9" s="11"/>
-      <c r="AF9" s="11"/>
-      <c r="AG9" s="11" t="s">
+      <c r="R9" s="9"/>
+      <c r="S9" s="9"/>
+      <c r="T9" s="9"/>
+      <c r="U9" s="9"/>
+      <c r="V9" s="9"/>
+      <c r="W9" s="9"/>
+      <c r="X9" s="9"/>
+      <c r="Y9" s="9"/>
+      <c r="Z9" s="9"/>
+      <c r="AA9" s="9"/>
+      <c r="AB9" s="9"/>
+      <c r="AC9" s="9"/>
+      <c r="AD9" s="9"/>
+      <c r="AE9" s="9"/>
+      <c r="AF9" s="9"/>
+      <c r="AG9" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="AH9" s="11" t="s">
+      <c r="AH9" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="AI9" s="11" t="s">
+      <c r="AI9" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="AJ9" s="11" t="s">
+      <c r="AJ9" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="AK9" s="11" t="s">
+      <c r="AK9" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="AL9" s="11" t="s">
+      <c r="AL9" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="AM9" s="11" t="s">
+      <c r="AM9" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="AN9" s="11" t="s">
+      <c r="AN9" s="19"/>
+      <c r="AO9" s="19"/>
+      <c r="AP9" s="19"/>
+      <c r="AQ9" s="19"/>
+      <c r="AR9" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="AO9" s="16" t="s">
+      <c r="AS9" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="AP9" s="16"/>
-      <c r="AQ9" s="16"/>
-      <c r="AR9" s="16"/>
-      <c r="AS9" s="16"/>
-      <c r="AT9" s="16"/>
-      <c r="AU9" s="11" t="s">
+      <c r="AT9" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="AV9" s="11" t="s">
+      <c r="AU9" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="AW9" s="11" t="s">
+      <c r="AV9" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="AX9" s="11" t="s">
+      <c r="AW9" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="AY9" s="11" t="s">
+    </row>
+    <row r="10" spans="1:49" ht="26.1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="10"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="12"/>
+      <c r="L10" s="12"/>
+      <c r="M10" s="12"/>
+      <c r="N10" s="12"/>
+      <c r="O10" s="12"/>
+      <c r="P10" s="13"/>
+      <c r="Q10" s="11"/>
+      <c r="R10" s="12"/>
+      <c r="S10" s="12"/>
+      <c r="T10" s="12"/>
+      <c r="U10" s="12"/>
+      <c r="V10" s="12"/>
+      <c r="W10" s="12"/>
+      <c r="X10" s="12"/>
+      <c r="Y10" s="12"/>
+      <c r="Z10" s="12"/>
+      <c r="AA10" s="12"/>
+      <c r="AB10" s="12"/>
+      <c r="AC10" s="12"/>
+      <c r="AD10" s="12"/>
+      <c r="AE10" s="12"/>
+      <c r="AF10" s="13"/>
+      <c r="AG10" s="10"/>
+      <c r="AH10" s="10"/>
+      <c r="AI10" s="10"/>
+      <c r="AJ10" s="10"/>
+      <c r="AK10" s="10"/>
+      <c r="AL10" s="10"/>
+      <c r="AM10" s="10"/>
+      <c r="AN10" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="AZ9" s="11" t="s">
+      <c r="AO10" s="4" t="s">
         <v>23</v>
       </c>
+      <c r="AP10" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="AQ10" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="AR10" s="10"/>
+      <c r="AS10" s="10"/>
+      <c r="AT10" s="10"/>
+      <c r="AU10" s="10"/>
+      <c r="AV10" s="10"/>
+      <c r="AW10" s="10"/>
     </row>
-    <row r="10" spans="1:52" ht="26" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="12"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="14"/>
-      <c r="L10" s="14"/>
-      <c r="M10" s="14"/>
-      <c r="N10" s="14"/>
-      <c r="O10" s="14"/>
-      <c r="P10" s="15"/>
-      <c r="Q10" s="13"/>
-      <c r="R10" s="14"/>
-      <c r="S10" s="14"/>
-      <c r="T10" s="14"/>
-      <c r="U10" s="14"/>
-      <c r="V10" s="14"/>
-      <c r="W10" s="14"/>
-      <c r="X10" s="14"/>
-      <c r="Y10" s="14"/>
-      <c r="Z10" s="14"/>
-      <c r="AA10" s="14"/>
-      <c r="AB10" s="14"/>
-      <c r="AC10" s="14"/>
-      <c r="AD10" s="14"/>
-      <c r="AE10" s="14"/>
-      <c r="AF10" s="15"/>
-      <c r="AG10" s="12"/>
-      <c r="AH10" s="12"/>
-      <c r="AI10" s="12"/>
-      <c r="AJ10" s="12"/>
-      <c r="AK10" s="12"/>
-      <c r="AL10" s="12"/>
-      <c r="AM10" s="12"/>
-      <c r="AN10" s="12"/>
-      <c r="AO10" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="AP10" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="AQ10" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="AR10" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="AS10" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="AT10" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="AU10" s="12"/>
-      <c r="AV10" s="12"/>
-      <c r="AW10" s="12"/>
-      <c r="AX10" s="12"/>
-      <c r="AY10" s="12"/>
-      <c r="AZ10" s="12"/>
-    </row>
-    <row r="11" spans="1:52" ht="11" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:49" ht="11.1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A11" s="5">
         <v>1</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="C11" s="17"/>
       <c r="D11" s="17"/>
@@ -1128,7 +1067,7 @@
       <c r="F11" s="17"/>
       <c r="G11" s="17"/>
       <c r="H11" s="17" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="I11" s="17"/>
       <c r="J11" s="17"/>
@@ -1139,7 +1078,7 @@
       <c r="O11" s="17"/>
       <c r="P11" s="17"/>
       <c r="Q11" s="18" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="R11" s="17"/>
       <c r="S11" s="17"/>
@@ -1160,67 +1099,58 @@
         <v>79998884455</v>
       </c>
       <c r="AH11" s="6" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="AI11" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="AJ11" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="AK11" s="19">
+        <v>48</v>
+      </c>
+      <c r="AJ11" s="8">
+        <v>44105</v>
+      </c>
+      <c r="AK11" s="8">
         <v>44835</v>
       </c>
-      <c r="AL11" s="6" t="s">
-        <v>31</v>
+      <c r="AL11" s="8">
+        <v>34894</v>
       </c>
       <c r="AM11" s="6" t="s">
         <v>32</v>
       </c>
       <c r="AN11" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="AO11" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="AP11" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="AQ11" s="6">
+        <v>37</v>
+      </c>
+      <c r="AO11" s="6">
         <v>123456</v>
       </c>
+      <c r="AP11" s="8">
+        <v>43690</v>
+      </c>
+      <c r="AQ11" s="6" t="s">
+        <v>38</v>
+      </c>
       <c r="AR11" s="6" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="AS11" s="6" t="s">
-        <v>51</v>
+        <v>27</v>
       </c>
       <c r="AT11" s="6" t="s">
-        <v>52</v>
+        <v>28</v>
       </c>
       <c r="AU11" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="AV11" s="6" t="s">
-        <v>37</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="AV11" s="7"/>
       <c r="AW11" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="AX11" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="AY11" s="7"/>
-      <c r="AZ11" s="6" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:52" ht="22.05" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:49" ht="22.15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A12" s="5">
         <v>2</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="C12" s="17"/>
       <c r="D12" s="17"/>
@@ -1228,7 +1158,7 @@
       <c r="F12" s="17"/>
       <c r="G12" s="17"/>
       <c r="H12" s="17" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="I12" s="17"/>
       <c r="J12" s="17"/>
@@ -1239,7 +1169,7 @@
       <c r="O12" s="17"/>
       <c r="P12" s="17"/>
       <c r="Q12" s="18" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="R12" s="17"/>
       <c r="S12" s="17"/>
@@ -1258,63 +1188,52 @@
       <c r="AF12" s="17"/>
       <c r="AG12" s="6"/>
       <c r="AH12" s="6" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="AI12" s="6" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="AJ12" s="6" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="AK12" s="6"/>
       <c r="AL12" s="6" t="s">
         <v>31</v>
       </c>
       <c r="AM12" s="6" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="AN12" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="AO12" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AO12" s="6">
+        <v>859173</v>
+      </c>
+      <c r="AP12" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="AQ12" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="AR12" s="6"/>
+      <c r="AS12" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="AP12" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="AQ12" s="6">
-        <v>859173</v>
-      </c>
-      <c r="AR12" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="AS12" s="6" t="s">
-        <v>36</v>
-      </c>
       <c r="AT12" s="6" t="s">
-        <v>66</v>
+        <v>28</v>
       </c>
       <c r="AU12" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="AV12" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="AW12" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="AX12" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="AY12" s="6"/>
-      <c r="AZ12" s="6"/>
+        <v>29</v>
+      </c>
+      <c r="AV12" s="6"/>
+      <c r="AW12" s="6"/>
     </row>
-    <row r="13" spans="1:52" ht="22.05" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:49" ht="22.15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A13" s="5">
         <v>3</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="C13" s="17"/>
       <c r="D13" s="17"/>
@@ -1322,7 +1241,7 @@
       <c r="F13" s="17"/>
       <c r="G13" s="17"/>
       <c r="H13" s="17" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="I13" s="17"/>
       <c r="J13" s="17"/>
@@ -1333,7 +1252,7 @@
       <c r="O13" s="17"/>
       <c r="P13" s="17"/>
       <c r="Q13" s="18" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="R13" s="17"/>
       <c r="S13" s="17"/>
@@ -1354,74 +1273,61 @@
         <v>79998884455</v>
       </c>
       <c r="AH13" s="6" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="AI13" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="AJ13" s="6" t="s">
-        <v>45</v>
+        <v>50</v>
+      </c>
+      <c r="AJ13" s="8">
+        <v>44648</v>
       </c>
       <c r="AK13" s="6"/>
-      <c r="AL13" s="6" t="s">
-        <v>31</v>
+      <c r="AL13" s="8">
+        <v>34128</v>
       </c>
       <c r="AM13" s="6" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="AN13" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="AO13" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="AP13" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="AQ13" s="6">
+        <v>57</v>
+      </c>
+      <c r="AO13" s="6">
         <v>563732</v>
       </c>
+      <c r="AP13" s="8">
+        <v>44824</v>
+      </c>
+      <c r="AQ13" s="6" t="s">
+        <v>26</v>
+      </c>
       <c r="AR13" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="AS13" s="6" t="s">
-        <v>36</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="AS13" s="6"/>
       <c r="AT13" s="6" t="s">
-        <v>67</v>
+        <v>28</v>
       </c>
       <c r="AU13" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="AV13" s="6"/>
+        <v>29</v>
+      </c>
+      <c r="AV13" s="5">
+        <v>1</v>
+      </c>
       <c r="AW13" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="AX13" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="AY13" s="5">
-        <v>1</v>
-      </c>
-      <c r="AZ13" s="6" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:52" s="1" customFormat="1" ht="10.050000000000001" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:49" s="1" customFormat="1" ht="10.15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="33">
+  <mergeCells count="32">
+    <mergeCell ref="AV9:AV10"/>
     <mergeCell ref="B12:G12"/>
     <mergeCell ref="H12:P12"/>
     <mergeCell ref="Q12:AF12"/>
     <mergeCell ref="B13:G13"/>
     <mergeCell ref="H13:P13"/>
     <mergeCell ref="Q13:AF13"/>
-    <mergeCell ref="AU9:AU10"/>
-    <mergeCell ref="AV9:AV10"/>
     <mergeCell ref="AW9:AW10"/>
-    <mergeCell ref="AX9:AX10"/>
-    <mergeCell ref="AY9:AY10"/>
-    <mergeCell ref="AZ9:AZ10"/>
     <mergeCell ref="B11:G11"/>
     <mergeCell ref="H11:P11"/>
     <mergeCell ref="Q11:AF11"/>
@@ -1432,17 +1338,20 @@
     <mergeCell ref="AK9:AK10"/>
     <mergeCell ref="AL9:AL10"/>
     <mergeCell ref="AM9:AM10"/>
-    <mergeCell ref="AN9:AN10"/>
-    <mergeCell ref="AO9:AT9"/>
+    <mergeCell ref="AN9:AQ9"/>
+    <mergeCell ref="AR9:AR10"/>
+    <mergeCell ref="AS9:AS10"/>
+    <mergeCell ref="AT9:AT10"/>
+    <mergeCell ref="AU9:AU10"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:G10"/>
+    <mergeCell ref="H9:P10"/>
+    <mergeCell ref="Q9:AF10"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="A6:D6"/>
     <mergeCell ref="E6:AE6"/>
     <mergeCell ref="A7:D7"/>
     <mergeCell ref="E7:AE8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:G10"/>
-    <mergeCell ref="H9:P10"/>
-    <mergeCell ref="Q9:AF10"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
Fix column names in employee import config
</commit_message>
<xml_diff>
--- a/platform/src/test/resources/excel/employees-to-import.xlsx
+++ b/platform/src/test/resources/excel/employees-to-import.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="71">
   <si>
     <t xml:space="preserve">Личные данные сотрудников</t>
   </si>
@@ -68,12 +68,18 @@
     <t xml:space="preserve">Дата увольнения</t>
   </si>
   <si>
+    <t xml:space="preserve">График работы</t>
+  </si>
+  <si>
     <t xml:space="preserve">Дата рождения</t>
   </si>
   <si>
     <t xml:space="preserve">Пол</t>
   </si>
   <si>
+    <t xml:space="preserve">Удостоверение личности</t>
+  </si>
+  <si>
     <t xml:space="preserve">Адрес места проживания</t>
   </si>
   <si>
@@ -92,6 +98,9 @@
     <t xml:space="preserve">Состав семьи</t>
   </si>
   <si>
+    <t xml:space="preserve">Вид</t>
+  </si>
+  <si>
     <t xml:space="preserve">Серия</t>
   </si>
   <si>
@@ -102,6 +111,9 @@
   </si>
   <si>
     <t xml:space="preserve">Кем выдано</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Код подразделения</t>
   </si>
   <si>
     <t xml:space="preserve">Хайден Спуннер </t>
@@ -346,7 +358,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -379,6 +391,14 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -392,10 +412,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -485,13 +501,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:AW14"/>
+  <dimension ref="A1:AZ14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AH1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AK18" activeCellId="0" sqref="AK18"/>
+      <selection pane="topLeft" activeCell="AQ21" activeCellId="0" sqref="AQ21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5078125" defaultRowHeight="11.25" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="5.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="3.66"/>
@@ -512,16 +528,16 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="1" width="21.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="1" width="52.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="1" width="35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="36" style="1" width="14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="1" width="10.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="1" width="9.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="1" width="11.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="1" width="14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="43" style="1" width="74.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="45" min="45" style="1" width="57.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="46" style="1" width="17.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="48" style="1" width="14.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="49" style="1" width="74.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="36" style="1" width="14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="1" width="10.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="41" style="1" width="9.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="43" style="1" width="11.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="1" width="14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="45" style="1" width="74.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="48" style="1" width="57.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="50" min="49" style="1" width="17.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="51" min="51" style="1" width="14.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="52" min="52" style="1" width="74.67"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="9.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -718,33 +734,40 @@
       <c r="AK9" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="AL9" s="7" t="s">
+      <c r="AL9" s="8" t="s">
         <v>15</v>
       </c>
       <c r="AM9" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="AN9" s="7"/>
-      <c r="AO9" s="7"/>
-      <c r="AP9" s="7"/>
-      <c r="AQ9" s="7"/>
-      <c r="AR9" s="7" t="s">
+      <c r="AN9" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="AS9" s="7" t="s">
+      <c r="AO9" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="AT9" s="7" t="s">
+      <c r="AP9" s="8"/>
+      <c r="AQ9" s="8"/>
+      <c r="AR9" s="8"/>
+      <c r="AS9" s="8"/>
+      <c r="AT9" s="7"/>
+      <c r="AU9" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="AU9" s="7" t="s">
+      <c r="AV9" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="AV9" s="7" t="s">
+      <c r="AW9" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="AW9" s="7" t="s">
+      <c r="AX9" s="7" t="s">
         <v>22</v>
+      </c>
+      <c r="AY9" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="AZ9" s="7" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
@@ -787,291 +810,307 @@
       <c r="AK10" s="7"/>
       <c r="AL10" s="7"/>
       <c r="AM10" s="7"/>
-      <c r="AN10" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="AO10" s="7" t="s">
-        <v>24</v>
+      <c r="AN10" s="7"/>
+      <c r="AO10" s="9" t="s">
+        <v>25</v>
       </c>
       <c r="AP10" s="7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="AQ10" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="AR10" s="7"/>
-      <c r="AS10" s="7"/>
-      <c r="AT10" s="7"/>
+        <v>27</v>
+      </c>
+      <c r="AR10" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="AS10" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="AT10" s="9" t="s">
+        <v>30</v>
+      </c>
       <c r="AU10" s="7"/>
       <c r="AV10" s="7"/>
       <c r="AW10" s="7"/>
+      <c r="AX10" s="7"/>
+      <c r="AY10" s="7"/>
+      <c r="AZ10" s="7"/>
     </row>
     <row r="11" customFormat="false" ht="10.5" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
-      <c r="A11" s="8" t="n">
+      <c r="A11" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="B11" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9"/>
-      <c r="K11" s="9"/>
-      <c r="L11" s="9"/>
-      <c r="M11" s="9"/>
-      <c r="N11" s="9"/>
-      <c r="O11" s="9"/>
-      <c r="P11" s="9"/>
-      <c r="Q11" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="R11" s="10"/>
-      <c r="S11" s="10"/>
-      <c r="T11" s="10"/>
-      <c r="U11" s="10"/>
-      <c r="V11" s="10"/>
-      <c r="W11" s="10"/>
-      <c r="X11" s="10"/>
-      <c r="Y11" s="10"/>
-      <c r="Z11" s="10"/>
-      <c r="AA11" s="10"/>
-      <c r="AB11" s="10"/>
-      <c r="AC11" s="10"/>
-      <c r="AD11" s="10"/>
-      <c r="AE11" s="10"/>
-      <c r="AF11" s="10"/>
-      <c r="AG11" s="9" t="n">
+      <c r="B11" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
+      <c r="M11" s="11"/>
+      <c r="N11" s="11"/>
+      <c r="O11" s="11"/>
+      <c r="P11" s="11"/>
+      <c r="Q11" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="R11" s="12"/>
+      <c r="S11" s="12"/>
+      <c r="T11" s="12"/>
+      <c r="U11" s="12"/>
+      <c r="V11" s="12"/>
+      <c r="W11" s="12"/>
+      <c r="X11" s="12"/>
+      <c r="Y11" s="12"/>
+      <c r="Z11" s="12"/>
+      <c r="AA11" s="12"/>
+      <c r="AB11" s="12"/>
+      <c r="AC11" s="12"/>
+      <c r="AD11" s="12"/>
+      <c r="AE11" s="12"/>
+      <c r="AF11" s="12"/>
+      <c r="AG11" s="11" t="n">
         <v>79998884455</v>
       </c>
-      <c r="AH11" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="AI11" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="AJ11" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="AK11" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="AL11" s="11" t="s">
+      <c r="AH11" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="AM11" s="9" t="s">
+      <c r="AI11" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="AN11" s="9" t="s">
+      <c r="AJ11" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="AO11" s="9" t="n">
+      <c r="AK11" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="AL11" s="11"/>
+      <c r="AM11" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="AN11" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="AO11" s="11"/>
+      <c r="AP11" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="AQ11" s="11" t="n">
         <v>123456</v>
       </c>
-      <c r="AP11" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="AQ11" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="AR11" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="AS11" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="AT11" s="9" t="s">
+      <c r="AR11" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="AU11" s="9" t="s">
+      <c r="AS11" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="AV11" s="14"/>
-      <c r="AW11" s="9" t="s">
+      <c r="AT11" s="11"/>
+      <c r="AU11" s="11" t="s">
         <v>43</v>
+      </c>
+      <c r="AV11" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="AW11" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="AX11" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="AY11" s="15"/>
+      <c r="AZ11" s="11" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
-      <c r="A12" s="8" t="n">
+      <c r="A12" s="10" t="n">
         <v>2</v>
       </c>
-      <c r="B12" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9" t="s">
+      <c r="B12" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="11"/>
+      <c r="M12" s="11"/>
+      <c r="N12" s="11"/>
+      <c r="O12" s="11"/>
+      <c r="P12" s="11"/>
+      <c r="Q12" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="R12" s="12"/>
+      <c r="S12" s="12"/>
+      <c r="T12" s="12"/>
+      <c r="U12" s="12"/>
+      <c r="V12" s="12"/>
+      <c r="W12" s="12"/>
+      <c r="X12" s="12"/>
+      <c r="Y12" s="12"/>
+      <c r="Z12" s="12"/>
+      <c r="AA12" s="12"/>
+      <c r="AB12" s="12"/>
+      <c r="AC12" s="12"/>
+      <c r="AD12" s="12"/>
+      <c r="AE12" s="12"/>
+      <c r="AF12" s="12"/>
+      <c r="AG12" s="11"/>
+      <c r="AH12" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="AI12" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="AJ12" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="AK12" s="11"/>
+      <c r="AL12" s="11"/>
+      <c r="AM12" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="AN12" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="AO12" s="11"/>
+      <c r="AP12" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AQ12" s="11" t="n">
+        <v>859173</v>
+      </c>
+      <c r="AR12" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="AS12" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="AT12" s="11"/>
+      <c r="AU12" s="11"/>
+      <c r="AV12" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="AW12" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="I12" s="9"/>
-      <c r="J12" s="9"/>
-      <c r="K12" s="9"/>
-      <c r="L12" s="9"/>
-      <c r="M12" s="9"/>
-      <c r="N12" s="9"/>
-      <c r="O12" s="9"/>
-      <c r="P12" s="9"/>
-      <c r="Q12" s="10" t="s">
+      <c r="AX12" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="R12" s="10"/>
-      <c r="S12" s="10"/>
-      <c r="T12" s="10"/>
-      <c r="U12" s="10"/>
-      <c r="V12" s="10"/>
-      <c r="W12" s="10"/>
-      <c r="X12" s="10"/>
-      <c r="Y12" s="10"/>
-      <c r="Z12" s="10"/>
-      <c r="AA12" s="10"/>
-      <c r="AB12" s="10"/>
-      <c r="AC12" s="10"/>
-      <c r="AD12" s="10"/>
-      <c r="AE12" s="10"/>
-      <c r="AF12" s="10"/>
-      <c r="AG12" s="9"/>
-      <c r="AH12" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="AI12" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="AJ12" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="AK12" s="9"/>
-      <c r="AL12" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="AM12" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="AN12" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="AO12" s="9" t="n">
-        <v>859173</v>
-      </c>
-      <c r="AP12" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="AQ12" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="AR12" s="9"/>
-      <c r="AS12" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="AT12" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="AU12" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="AV12" s="9"/>
-      <c r="AW12" s="9"/>
+      <c r="AY12" s="11"/>
+      <c r="AZ12" s="11"/>
     </row>
     <row r="13" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
-      <c r="A13" s="8" t="n">
+      <c r="A13" s="10" t="n">
         <v>3</v>
       </c>
-      <c r="B13" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="I13" s="9"/>
-      <c r="J13" s="9"/>
-      <c r="K13" s="9"/>
-      <c r="L13" s="9"/>
-      <c r="M13" s="9"/>
-      <c r="N13" s="9"/>
-      <c r="O13" s="9"/>
-      <c r="P13" s="9"/>
-      <c r="Q13" s="10" t="s">
+      <c r="B13" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="I13" s="11"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="11"/>
+      <c r="M13" s="11"/>
+      <c r="N13" s="11"/>
+      <c r="O13" s="11"/>
+      <c r="P13" s="11"/>
+      <c r="Q13" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="R13" s="12"/>
+      <c r="S13" s="12"/>
+      <c r="T13" s="12"/>
+      <c r="U13" s="12"/>
+      <c r="V13" s="12"/>
+      <c r="W13" s="12"/>
+      <c r="X13" s="12"/>
+      <c r="Y13" s="12"/>
+      <c r="Z13" s="12"/>
+      <c r="AA13" s="12"/>
+      <c r="AB13" s="12"/>
+      <c r="AC13" s="12"/>
+      <c r="AD13" s="12"/>
+      <c r="AE13" s="12"/>
+      <c r="AF13" s="12"/>
+      <c r="AG13" s="11" t="n">
+        <v>79998884455</v>
+      </c>
+      <c r="AH13" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="AI13" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="AJ13" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="AK13" s="11"/>
+      <c r="AL13" s="11"/>
+      <c r="AM13" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="AN13" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="AO13" s="11"/>
+      <c r="AP13" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="AQ13" s="11" t="n">
+        <v>563732</v>
+      </c>
+      <c r="AR13" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="AS13" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="R13" s="10"/>
-      <c r="S13" s="10"/>
-      <c r="T13" s="10"/>
-      <c r="U13" s="10"/>
-      <c r="V13" s="10"/>
-      <c r="W13" s="10"/>
-      <c r="X13" s="10"/>
-      <c r="Y13" s="10"/>
-      <c r="Z13" s="10"/>
-      <c r="AA13" s="10"/>
-      <c r="AB13" s="10"/>
-      <c r="AC13" s="10"/>
-      <c r="AD13" s="10"/>
-      <c r="AE13" s="10"/>
-      <c r="AF13" s="10"/>
-      <c r="AG13" s="9" t="n">
-        <v>79998884455</v>
-      </c>
-      <c r="AH13" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="AI13" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="AJ13" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="AK13" s="9"/>
-      <c r="AL13" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="AM13" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="AN13" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="AO13" s="9" t="n">
-        <v>563732</v>
-      </c>
-      <c r="AP13" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="AQ13" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="AR13" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="AS13" s="9"/>
-      <c r="AT13" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="AU13" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="AV13" s="8" t="n">
+      <c r="AT13" s="11"/>
+      <c r="AU13" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="AV13" s="11"/>
+      <c r="AW13" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="AX13" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="AY13" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="AW13" s="9" t="s">
-        <v>66</v>
+      <c r="AZ13" s="11" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="true" ht="9.75" hidden="false" customHeight="true" outlineLevel="1" collapsed="false"/>
   </sheetData>
-  <mergeCells count="32">
+  <mergeCells count="33">
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="A6:D6"/>
     <mergeCell ref="E6:AE6"/>
@@ -1088,13 +1127,14 @@
     <mergeCell ref="AK9:AK10"/>
     <mergeCell ref="AL9:AL10"/>
     <mergeCell ref="AM9:AM10"/>
-    <mergeCell ref="AN9:AQ9"/>
-    <mergeCell ref="AR9:AR10"/>
-    <mergeCell ref="AS9:AS10"/>
-    <mergeCell ref="AT9:AT10"/>
+    <mergeCell ref="AN9:AN10"/>
+    <mergeCell ref="AO9:AS9"/>
     <mergeCell ref="AU9:AU10"/>
     <mergeCell ref="AV9:AV10"/>
     <mergeCell ref="AW9:AW10"/>
+    <mergeCell ref="AX9:AX10"/>
+    <mergeCell ref="AY9:AY10"/>
+    <mergeCell ref="AZ9:AZ10"/>
     <mergeCell ref="B11:G11"/>
     <mergeCell ref="H11:P11"/>
     <mergeCell ref="Q11:AF11"/>

</xml_diff>